<commit_message>
add box plots; styling 1
</commit_message>
<xml_diff>
--- a/tests/assets/Test Mini HOLPA Household Survey.xlsx
+++ b/tests/assets/Test Mini HOLPA Household Survey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dave/Sites/holpa-platform/tests/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A021BCB-9E77-2B42-8CED-916E0571423C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D88387-1B88-E54E-B1EA-E5ECBB14C579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-300" yWindow="8860" windowWidth="30240" windowHeight="18880" tabRatio="321" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="8860" windowWidth="30240" windowHeight="18880" tabRatio="321" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -105,9 +105,6 @@
     <t>list_name</t>
   </si>
   <si>
-    <t>media::image</t>
-  </si>
-  <si>
     <t>default_language</t>
   </si>
   <si>
@@ -448,6 +445,9 @@
   </si>
   <si>
     <t>test_holpa_household</t>
+  </si>
+  <si>
+    <t>media::image::English (en)</t>
   </si>
 </sst>
 </file>
@@ -1343,9 +1343,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView zoomScale="156" zoomScaleNormal="90" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="156" zoomScaleNormal="90" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
+      <selection pane="bottomLeft" activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.6640625" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1368,7 +1368,7 @@
   <sheetData>
     <row r="1" spans="1:15" s="15" customFormat="1" ht="38" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>0</v>
@@ -1377,10 +1377,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="17" t="s">
         <v>99</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>100</v>
       </c>
       <c r="F1" s="15" t="s">
         <v>2</v>
@@ -1398,7 +1398,7 @@
         <v>4</v>
       </c>
       <c r="K1" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L1" s="15" t="s">
         <v>6</v>
@@ -1407,7 +1407,7 @@
         <v>18</v>
       </c>
       <c r="N1" s="20" t="s">
-        <v>20</v>
+        <v>134</v>
       </c>
       <c r="O1" s="18" t="s">
         <v>8</v>
@@ -1415,16 +1415,16 @@
     </row>
     <row r="2" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E2" s="11"/>
       <c r="H2" s="8"/>
@@ -1434,19 +1434,19 @@
     </row>
     <row r="3" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H3" s="8"/>
       <c r="K3" s="9"/>
@@ -1455,19 +1455,19 @@
     </row>
     <row r="4" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H4" s="8"/>
       <c r="K4" s="9"/>
@@ -1476,16 +1476,16 @@
     </row>
     <row r="5" spans="1:15" s="7" customFormat="1" ht="35" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>106</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>107</v>
       </c>
       <c r="E5" s="11"/>
       <c r="H5" s="8"/>
@@ -1495,19 +1495,19 @@
     </row>
     <row r="6" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="11"/>
       <c r="H6" s="8"/>
       <c r="I6" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K6" s="9"/>
       <c r="M6" s="10"/>
@@ -1515,256 +1515,256 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" s="12" t="s">
         <v>26</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="J9" s="1" t="s">
+      <c r="K9" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="23" t="s">
         <v>32</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>33</v>
       </c>
       <c r="E10" s="24"/>
       <c r="F10" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G10" s="23"/>
       <c r="N10" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E11" s="24"/>
       <c r="F11" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G11" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B12" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="D12" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="E12" s="26" t="s">
         <v>41</v>
-      </c>
-      <c r="E12" s="26" t="s">
-        <v>42</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="23"/>
     </row>
     <row r="13" spans="1:15" ht="20" x14ac:dyDescent="0.25">
       <c r="A13" s="28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E13" s="26"/>
       <c r="F13" s="23"/>
       <c r="G13" s="23"/>
       <c r="M13" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B14" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="25" t="s">
         <v>67</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>68</v>
       </c>
       <c r="D14" s="26"/>
       <c r="E14" s="26"/>
       <c r="F14" s="23"/>
       <c r="G14" s="23"/>
       <c r="I14" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B15" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="25" t="s">
         <v>63</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>64</v>
       </c>
       <c r="D15" s="26"/>
       <c r="E15" s="26"/>
       <c r="F15" s="23"/>
       <c r="G15" s="23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D16" s="26"/>
       <c r="E16" s="26"/>
       <c r="F16" s="23"/>
       <c r="G16" s="23"/>
       <c r="I16" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="40" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E17" s="26"/>
       <c r="F17" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G17" s="23"/>
     </row>
     <row r="18" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="26" t="s">
+      <c r="E18" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="E18" s="26" t="s">
-        <v>84</v>
-      </c>
       <c r="F18" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G18" s="23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A19" s="28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E19" s="26"/>
       <c r="F19" s="23"/>
@@ -1772,34 +1772,34 @@
     </row>
     <row r="20" spans="1:7" ht="80" x14ac:dyDescent="0.25">
       <c r="A20" s="28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="D20" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="D20" s="26" t="s">
-        <v>120</v>
-      </c>
       <c r="E20" s="26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F20" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G20" s="23"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D21" s="26"/>
       <c r="E21" s="26"/>
@@ -1808,13 +1808,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D22" s="26"/>
       <c r="E22" s="26"/>
@@ -1823,13 +1823,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D23" s="26"/>
       <c r="E23" s="26"/>
@@ -1841,19 +1841,19 @@
         <v>13</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="E24" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="E24" s="24" t="s">
-        <v>48</v>
-      </c>
       <c r="F24" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G24" s="23"/>
     </row>
@@ -1862,22 +1862,22 @@
         <v>13</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D25" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="E25" s="24" t="s">
+      <c r="F25" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G25" s="23" t="s">
         <v>50</v>
-      </c>
-      <c r="F25" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="G25" s="23" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1885,16 +1885,16 @@
         <v>13</v>
       </c>
       <c r="B26" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="23" t="s">
+      <c r="D26" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="23" t="s">
-        <v>45</v>
-      </c>
       <c r="E26" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F26" s="23"/>
       <c r="G26" s="23"/>
@@ -1904,16 +1904,16 @@
         <v>13</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C27" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="D27" s="23" t="s">
+      <c r="E27" s="24" t="s">
         <v>57</v>
-      </c>
-      <c r="E27" s="24" t="s">
-        <v>58</v>
       </c>
       <c r="F27" s="23"/>
       <c r="G27" s="23"/>
@@ -1997,7 +1997,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="13" customFormat="1" ht="38" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>19</v>
@@ -2006,99 +2006,99 @@
         <v>1</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" s="14">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="14">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" t="s">
         <v>110</v>
-      </c>
-      <c r="D7" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" t="s">
         <v>112</v>
-      </c>
-      <c r="D8" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" t="s">
         <v>116</v>
-      </c>
-      <c r="D10" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -2109,57 +2109,57 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2173,8 +2173,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2199,22 +2199,22 @@
         <v>17</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" t="s">
         <v>133</v>
-      </c>
-      <c r="B2" t="s">
-        <v>134</v>
       </c>
       <c r="D2" s="27">
         <f ca="1">NOW()</f>
-        <v>45664.705639930558</v>
+        <v>46014.688906944444</v>
       </c>
       <c r="E2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>